<commit_message>
removed plate 1 from Fig 5b, Suppl table 2
</commit_message>
<xml_diff>
--- a/SVGs/SupplTable_2.xlsx
+++ b/SVGs/SupplTable_2.xlsx
@@ -605,7 +605,7 @@
   <dimension ref="B1:AMJ15"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C3" activeCellId="0" sqref="C3"/>
+      <selection pane="topLeft" activeCell="G10" activeCellId="0" sqref="G10:I14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="17" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -690,7 +690,7 @@
         <v>8</v>
       </c>
       <c r="G5" s="16" t="n">
-        <v>67</v>
+        <v>49</v>
       </c>
       <c r="H5" s="17" t="n">
         <v>0</v>
@@ -700,13 +700,13 @@
       </c>
       <c r="J5" s="19" t="n">
         <f aca="false">SUM(G5:I5)</f>
-        <v>67</v>
+        <v>49</v>
       </c>
       <c r="K5" s="20"/>
       <c r="L5" s="20"/>
       <c r="M5" s="20"/>
     </row>
-    <row r="6" customFormat="false" ht="17" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B6" s="13"/>
       <c r="C6" s="13"/>
       <c r="D6" s="13"/>
@@ -715,7 +715,7 @@
         <v>9</v>
       </c>
       <c r="G6" s="22" t="n">
-        <v>43</v>
+        <v>29</v>
       </c>
       <c r="H6" s="23" t="n">
         <v>0</v>
@@ -725,13 +725,13 @@
       </c>
       <c r="J6" s="25" t="n">
         <f aca="false">SUM(G6:I6)</f>
-        <v>43</v>
+        <v>29</v>
       </c>
       <c r="K6" s="20"/>
       <c r="L6" s="20"/>
       <c r="M6" s="20"/>
     </row>
-    <row r="7" customFormat="false" ht="17" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B7" s="13"/>
       <c r="C7" s="13"/>
       <c r="D7" s="13"/>
@@ -746,17 +746,17 @@
         <v>0</v>
       </c>
       <c r="I7" s="24" t="n">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="J7" s="25" t="n">
         <f aca="false">SUM(G7:I7)</f>
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="K7" s="2"/>
       <c r="L7" s="2"/>
       <c r="M7" s="2"/>
     </row>
-    <row r="8" customFormat="false" ht="17" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B8" s="13"/>
       <c r="C8" s="14"/>
       <c r="D8" s="13"/>
@@ -781,7 +781,7 @@
       <c r="L8" s="2"/>
       <c r="M8" s="2"/>
     </row>
-    <row r="9" customFormat="false" ht="17" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B9" s="13"/>
       <c r="C9" s="14" t="s">
         <v>4</v>
@@ -825,7 +825,7 @@
         <v>8</v>
       </c>
       <c r="G10" s="16" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="H10" s="17" t="n">
         <v>0</v>
@@ -835,13 +835,13 @@
       </c>
       <c r="J10" s="36" t="n">
         <f aca="false">SUM(G10:I10)</f>
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="K10" s="2"/>
       <c r="L10" s="2"/>
       <c r="M10" s="2"/>
     </row>
-    <row r="11" customFormat="false" ht="17" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B11" s="13"/>
       <c r="C11" s="13"/>
       <c r="D11" s="13"/>
@@ -866,7 +866,7 @@
       <c r="L11" s="2"/>
       <c r="M11" s="2"/>
     </row>
-    <row r="12" customFormat="false" ht="17" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B12" s="13"/>
       <c r="C12" s="13"/>
       <c r="D12" s="13"/>
@@ -875,23 +875,23 @@
         <v>10</v>
       </c>
       <c r="G12" s="22" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H12" s="23" t="n">
         <v>2</v>
       </c>
       <c r="I12" s="24" t="n">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="J12" s="25" t="n">
         <f aca="false">SUM(G12:I12)</f>
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="K12" s="2"/>
       <c r="L12" s="2"/>
       <c r="M12" s="2"/>
     </row>
-    <row r="13" customFormat="false" ht="17" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B13" s="13"/>
       <c r="C13" s="14"/>
       <c r="D13" s="13"/>
@@ -916,7 +916,7 @@
       <c r="L13" s="2"/>
       <c r="M13" s="2"/>
     </row>
-    <row r="14" customFormat="false" ht="17" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B14" s="13"/>
       <c r="C14" s="14"/>
       <c r="D14" s="13"/>
@@ -933,11 +933,11 @@
         <v>12</v>
       </c>
       <c r="I14" s="34" t="n">
-        <v>695</v>
+        <v>647</v>
       </c>
       <c r="J14" s="35" t="n">
         <f aca="false">SUM(G14:I14)</f>
-        <v>709</v>
+        <v>661</v>
       </c>
       <c r="K14" s="2"/>
       <c r="L14" s="2"/>
@@ -949,7 +949,7 @@
       </c>
       <c r="G15" s="28" t="n">
         <f aca="false">SUM(G5:G14)</f>
-        <v>126</v>
+        <v>90</v>
       </c>
       <c r="H15" s="28" t="n">
         <f aca="false">SUM(H5:H14)</f>
@@ -957,11 +957,11 @@
       </c>
       <c r="I15" s="28" t="n">
         <f aca="false">SUM(I5:I14)</f>
-        <v>743</v>
+        <v>684</v>
       </c>
       <c r="J15" s="39" t="n">
         <f aca="false">SUM(G15:I15)</f>
-        <v>884</v>
+        <v>789</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
removed stratification by 'inconclusive' samples, just 'pos' and 'neg' now
</commit_message>
<xml_diff>
--- a/SVGs/SupplTable_2.xlsx
+++ b/SVGs/SupplTable_2.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="11">
   <si>
     <t xml:space="preserve">RT-LAMP
 Result </t>
@@ -30,9 +30,6 @@
   </si>
   <si>
     <t xml:space="preserve">pos</t>
-  </si>
-  <si>
-    <t xml:space="preserve">inc.</t>
   </si>
   <si>
     <t xml:space="preserve">neg</t>
@@ -127,7 +124,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="30">
+  <borders count="28">
     <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
@@ -158,13 +155,6 @@
     </border>
     <border diagonalUp="false" diagonalDown="false">
       <left/>
-      <right/>
-      <top style="thin"/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left/>
       <right style="double"/>
       <top style="thin"/>
       <bottom/>
@@ -207,13 +197,6 @@
     </border>
     <border diagonalUp="false" diagonalDown="false">
       <left/>
-      <right/>
-      <top style="double"/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left/>
       <right style="double"/>
       <top style="double"/>
       <bottom/>
@@ -263,13 +246,6 @@
     </border>
     <border diagonalUp="false" diagonalDown="false">
       <left style="double"/>
-      <right/>
-      <top/>
-      <bottom style="thin"/>
-      <diagonal/>
-    </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left/>
       <right/>
       <top/>
       <bottom style="thin"/>
@@ -327,6 +303,13 @@
     <border diagonalUp="false" diagonalDown="false">
       <left style="thin"/>
       <right style="double"/>
+      <top/>
+      <bottom style="thin"/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left/>
+      <right/>
       <top/>
       <bottom style="thin"/>
       <diagonal/>
@@ -364,7 +347,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="35">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -381,10 +364,6 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -409,119 +388,103 @@
       <alignment horizontal="right" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="2" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="right" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="164" fontId="5" fillId="2" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="5" fillId="2" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="true" indent="0" shrinkToFit="false"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="5" fillId="2" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="2" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="2" borderId="12" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="2" borderId="14" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="2" borderId="16" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="16" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="17" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="2" borderId="18" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="17" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="18" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="2" borderId="19" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="19" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="20" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="164" fontId="5" fillId="2" borderId="20" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="21" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="2" borderId="22" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="22" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="23" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="24" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="25" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="2" borderId="23" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="24" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="22" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="25" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="165" fontId="4" fillId="0" borderId="26" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="4" fillId="0" borderId="27" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="28" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="29" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -605,65 +568,59 @@
   <dimension ref="B1:AMJ15"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G10" activeCellId="0" sqref="G10:I14"/>
+      <selection pane="topLeft" activeCell="G10" activeCellId="0" sqref="G10:H14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="17" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="1" width="7.26"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="10.12"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="7.26"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="5" style="1" width="10.12"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="6.67"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="6.94"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="7.92"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="7.26"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="10"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="1" width="4.17"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="1" width="8.61"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1016" min="14" style="1" width="11.52"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="1017" style="2" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="7.92"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="7.26"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="10"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="4.17"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="1" width="8.61"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1015" min="13" style="1" width="11.52"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1023" min="1016" style="2" width="11.52"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="17" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="G1" s="3"/>
       <c r="H1" s="4"/>
-      <c r="I1" s="5"/>
     </row>
     <row r="2" customFormat="false" ht="19" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G2" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="H2" s="6"/>
-      <c r="I2" s="6"/>
-    </row>
-    <row r="3" customFormat="false" ht="17" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="G3" s="6"/>
-      <c r="H3" s="6"/>
-      <c r="I3" s="6"/>
+      <c r="G2" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="H2" s="5"/>
+    </row>
+    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G3" s="5"/>
+      <c r="H3" s="5"/>
+      <c r="J3" s="2"/>
       <c r="K3" s="2"/>
       <c r="L3" s="2"/>
-      <c r="M3" s="2"/>
-    </row>
-    <row r="4" s="7" customFormat="true" ht="17" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F4" s="8" t="s">
+    </row>
+    <row r="4" s="6" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F4" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="G4" s="9" t="s">
+      <c r="G4" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="H4" s="10" t="s">
+      <c r="H4" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="I4" s="11" t="s">
+      <c r="I4" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="J4" s="12" t="s">
-        <v>5</v>
-      </c>
+      <c r="J4" s="2"/>
       <c r="K4" s="2"/>
       <c r="L4" s="2"/>
-      <c r="M4" s="2"/>
+      <c r="AMB4" s="2"/>
       <c r="AMC4" s="2"/>
       <c r="AMD4" s="2"/>
       <c r="AME4" s="2"/>
@@ -671,302 +628,268 @@
       <c r="AMG4" s="2"/>
       <c r="AMH4" s="2"/>
       <c r="AMI4" s="2"/>
-      <c r="AMJ4" s="2"/>
+      <c r="AMJ4" s="0"/>
     </row>
     <row r="5" customFormat="false" ht="19" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B5" s="13" t="s">
+      <c r="B5" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="C5" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="D5" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="14" t="s">
+      <c r="E5" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="D5" s="13" t="s">
+      <c r="F5" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="E5" s="14" t="s">
-        <v>2</v>
-      </c>
-      <c r="F5" s="15" t="s">
+      <c r="G5" s="14" t="n">
+        <v>49</v>
+      </c>
+      <c r="H5" s="15" t="n">
+        <v>0</v>
+      </c>
+      <c r="I5" s="16" t="n">
+        <f aca="false">SUM(G5:H5)</f>
+        <v>49</v>
+      </c>
+      <c r="J5" s="17"/>
+      <c r="K5" s="17"/>
+      <c r="L5" s="17"/>
+    </row>
+    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B6" s="11"/>
+      <c r="C6" s="11"/>
+      <c r="D6" s="11"/>
+      <c r="E6" s="11"/>
+      <c r="F6" s="18" t="s">
         <v>8</v>
       </c>
-      <c r="G5" s="16" t="n">
-        <v>49</v>
-      </c>
-      <c r="H5" s="17" t="n">
-        <v>0</v>
-      </c>
-      <c r="I5" s="18" t="n">
-        <v>0</v>
-      </c>
-      <c r="J5" s="19" t="n">
-        <f aca="false">SUM(G5:I5)</f>
-        <v>49</v>
-      </c>
-      <c r="K5" s="20"/>
-      <c r="L5" s="20"/>
-      <c r="M5" s="20"/>
-    </row>
-    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B6" s="13"/>
-      <c r="C6" s="13"/>
-      <c r="D6" s="13"/>
-      <c r="E6" s="13"/>
-      <c r="F6" s="21" t="s">
+      <c r="G6" s="19" t="n">
+        <v>29</v>
+      </c>
+      <c r="H6" s="20" t="n">
+        <v>0</v>
+      </c>
+      <c r="I6" s="21" t="n">
+        <f aca="false">SUM(G6:H6)</f>
+        <v>29</v>
+      </c>
+      <c r="J6" s="17"/>
+      <c r="K6" s="17"/>
+      <c r="L6" s="17"/>
+    </row>
+    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B7" s="11"/>
+      <c r="C7" s="11"/>
+      <c r="D7" s="11"/>
+      <c r="E7" s="11"/>
+      <c r="F7" s="18" t="s">
         <v>9</v>
       </c>
-      <c r="G6" s="22" t="n">
-        <v>29</v>
-      </c>
-      <c r="H6" s="23" t="n">
-        <v>0</v>
-      </c>
-      <c r="I6" s="24" t="n">
-        <v>0</v>
-      </c>
-      <c r="J6" s="25" t="n">
-        <f aca="false">SUM(G6:I6)</f>
-        <v>29</v>
-      </c>
-      <c r="K6" s="20"/>
-      <c r="L6" s="20"/>
-      <c r="M6" s="20"/>
-    </row>
-    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B7" s="13"/>
-      <c r="C7" s="13"/>
-      <c r="D7" s="13"/>
-      <c r="E7" s="13"/>
-      <c r="F7" s="21" t="s">
-        <v>10</v>
-      </c>
-      <c r="G7" s="22" t="n">
+      <c r="G7" s="19" t="n">
         <v>7</v>
       </c>
-      <c r="H7" s="23" t="n">
-        <v>0</v>
-      </c>
-      <c r="I7" s="24" t="n">
-        <v>0</v>
-      </c>
-      <c r="J7" s="25" t="n">
-        <f aca="false">SUM(G7:I7)</f>
+      <c r="H7" s="20" t="n">
+        <v>0</v>
+      </c>
+      <c r="I7" s="21" t="n">
+        <f aca="false">SUM(G7:H7)</f>
         <v>7</v>
       </c>
+      <c r="J7" s="2"/>
       <c r="K7" s="2"/>
       <c r="L7" s="2"/>
-      <c r="M7" s="2"/>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B8" s="13"/>
-      <c r="C8" s="14"/>
-      <c r="D8" s="13"/>
-      <c r="E8" s="14"/>
-      <c r="F8" s="26" t="s">
-        <v>11</v>
-      </c>
-      <c r="G8" s="27" t="n">
+      <c r="B8" s="11"/>
+      <c r="C8" s="12"/>
+      <c r="D8" s="11"/>
+      <c r="E8" s="12"/>
+      <c r="F8" s="22" t="s">
+        <v>10</v>
+      </c>
+      <c r="G8" s="23" t="n">
         <v>1</v>
       </c>
-      <c r="H8" s="28" t="n">
-        <v>0</v>
-      </c>
-      <c r="I8" s="29" t="n">
-        <v>0</v>
-      </c>
-      <c r="J8" s="25" t="n">
-        <f aca="false">SUM(G8:I8)</f>
+      <c r="H8" s="24" t="n">
+        <v>0</v>
+      </c>
+      <c r="I8" s="21" t="n">
+        <f aca="false">SUM(G8:H8)</f>
         <v>1</v>
       </c>
+      <c r="J8" s="2"/>
       <c r="K8" s="2"/>
       <c r="L8" s="2"/>
-      <c r="M8" s="2"/>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B9" s="13"/>
-      <c r="C9" s="14" t="s">
-        <v>4</v>
-      </c>
-      <c r="D9" s="13"/>
-      <c r="E9" s="30" t="s">
-        <v>4</v>
-      </c>
-      <c r="F9" s="31" t="s">
-        <v>4</v>
-      </c>
-      <c r="G9" s="32" t="n">
-        <v>0</v>
-      </c>
-      <c r="H9" s="33" t="n">
-        <v>0</v>
-      </c>
-      <c r="I9" s="34" t="n">
-        <v>0</v>
-      </c>
-      <c r="J9" s="35" t="n">
-        <f aca="false">SUM(G9:I9)</f>
-        <v>0</v>
-      </c>
+      <c r="B9" s="11"/>
+      <c r="C9" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="D9" s="11"/>
+      <c r="E9" s="25" t="s">
+        <v>3</v>
+      </c>
+      <c r="F9" s="26" t="s">
+        <v>3</v>
+      </c>
+      <c r="G9" s="27" t="n">
+        <v>0</v>
+      </c>
+      <c r="H9" s="28" t="n">
+        <v>0</v>
+      </c>
+      <c r="I9" s="29" t="n">
+        <f aca="false">SUM(G9:H9)</f>
+        <v>0</v>
+      </c>
+      <c r="J9" s="2"/>
       <c r="K9" s="2"/>
       <c r="L9" s="2"/>
-      <c r="M9" s="2"/>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B10" s="13"/>
-      <c r="C10" s="14" t="s">
-        <v>4</v>
-      </c>
-      <c r="D10" s="13" t="s">
+      <c r="B10" s="11"/>
+      <c r="C10" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="D10" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="E10" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="F10" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="E10" s="14" t="s">
+      <c r="G10" s="14" t="n">
         <v>2</v>
       </c>
-      <c r="F10" s="15" t="s">
-        <v>8</v>
-      </c>
-      <c r="G10" s="16" t="n">
+      <c r="H10" s="15" t="n">
+        <v>0</v>
+      </c>
+      <c r="I10" s="30" t="n">
+        <f aca="false">SUM(G10:H10)</f>
         <v>2</v>
       </c>
-      <c r="H10" s="17" t="n">
-        <v>0</v>
-      </c>
-      <c r="I10" s="18" t="n">
-        <v>0</v>
-      </c>
-      <c r="J10" s="36" t="n">
-        <f aca="false">SUM(G10:I10)</f>
-        <v>2</v>
-      </c>
+      <c r="J10" s="2"/>
       <c r="K10" s="2"/>
       <c r="L10" s="2"/>
-      <c r="M10" s="2"/>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B11" s="13"/>
-      <c r="C11" s="13"/>
-      <c r="D11" s="13"/>
-      <c r="E11" s="13"/>
-      <c r="F11" s="21" t="s">
-        <v>9</v>
-      </c>
-      <c r="G11" s="22" t="n">
-        <v>0</v>
-      </c>
-      <c r="H11" s="23" t="n">
-        <v>1</v>
-      </c>
-      <c r="I11" s="24" t="n">
-        <v>5</v>
-      </c>
-      <c r="J11" s="25" t="n">
-        <f aca="false">SUM(G11:I11)</f>
+      <c r="B11" s="11"/>
+      <c r="C11" s="11"/>
+      <c r="D11" s="11"/>
+      <c r="E11" s="11"/>
+      <c r="F11" s="18" t="s">
+        <v>8</v>
+      </c>
+      <c r="G11" s="19" t="n">
+        <v>0</v>
+      </c>
+      <c r="H11" s="20" t="n">
         <v>6</v>
       </c>
+      <c r="I11" s="21" t="n">
+        <f aca="false">SUM(G11:H11)</f>
+        <v>6</v>
+      </c>
+      <c r="J11" s="2"/>
       <c r="K11" s="2"/>
       <c r="L11" s="2"/>
-      <c r="M11" s="2"/>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B12" s="13"/>
-      <c r="C12" s="13"/>
-      <c r="D12" s="13"/>
-      <c r="E12" s="13"/>
-      <c r="F12" s="21" t="s">
-        <v>10</v>
-      </c>
-      <c r="G12" s="22" t="n">
-        <v>0</v>
-      </c>
-      <c r="H12" s="23" t="n">
-        <v>2</v>
-      </c>
-      <c r="I12" s="24" t="n">
-        <v>16</v>
-      </c>
-      <c r="J12" s="25" t="n">
-        <f aca="false">SUM(G12:I12)</f>
+      <c r="B12" s="11"/>
+      <c r="C12" s="11"/>
+      <c r="D12" s="11"/>
+      <c r="E12" s="11"/>
+      <c r="F12" s="18" t="s">
+        <v>9</v>
+      </c>
+      <c r="G12" s="19" t="n">
+        <v>0</v>
+      </c>
+      <c r="H12" s="20" t="n">
         <v>18</v>
       </c>
+      <c r="I12" s="21" t="n">
+        <f aca="false">SUM(G12:H12)</f>
+        <v>18</v>
+      </c>
+      <c r="J12" s="2"/>
       <c r="K12" s="2"/>
       <c r="L12" s="2"/>
-      <c r="M12" s="2"/>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B13" s="13"/>
-      <c r="C13" s="14"/>
-      <c r="D13" s="13"/>
-      <c r="E13" s="14"/>
-      <c r="F13" s="26" t="s">
-        <v>11</v>
-      </c>
-      <c r="G13" s="27" t="n">
-        <v>0</v>
-      </c>
-      <c r="H13" s="28" t="n">
-        <v>0</v>
-      </c>
-      <c r="I13" s="29" t="n">
+      <c r="B13" s="11"/>
+      <c r="C13" s="12"/>
+      <c r="D13" s="11"/>
+      <c r="E13" s="12"/>
+      <c r="F13" s="22" t="s">
+        <v>10</v>
+      </c>
+      <c r="G13" s="23" t="n">
+        <v>0</v>
+      </c>
+      <c r="H13" s="24" t="n">
         <v>16</v>
       </c>
-      <c r="J13" s="37" t="n">
-        <f aca="false">SUM(G13:I13)</f>
+      <c r="I13" s="31" t="n">
+        <f aca="false">SUM(G13:H13)</f>
         <v>16</v>
       </c>
+      <c r="J13" s="2"/>
       <c r="K13" s="2"/>
       <c r="L13" s="2"/>
-      <c r="M13" s="2"/>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B14" s="13"/>
-      <c r="C14" s="14"/>
-      <c r="D14" s="13"/>
-      <c r="E14" s="30" t="s">
-        <v>4</v>
-      </c>
-      <c r="F14" s="31" t="s">
-        <v>4</v>
-      </c>
-      <c r="G14" s="32" t="n">
+      <c r="B14" s="11"/>
+      <c r="C14" s="12"/>
+      <c r="D14" s="11"/>
+      <c r="E14" s="25" t="s">
+        <v>3</v>
+      </c>
+      <c r="F14" s="26" t="s">
+        <v>3</v>
+      </c>
+      <c r="G14" s="27" t="n">
         <v>2</v>
       </c>
-      <c r="H14" s="33" t="n">
-        <v>12</v>
-      </c>
-      <c r="I14" s="34" t="n">
-        <v>647</v>
-      </c>
-      <c r="J14" s="35" t="n">
-        <f aca="false">SUM(G14:I14)</f>
+      <c r="H14" s="28" t="n">
+        <v>659</v>
+      </c>
+      <c r="I14" s="29" t="n">
+        <f aca="false">SUM(G14:H14)</f>
         <v>661</v>
       </c>
+      <c r="J14" s="2"/>
       <c r="K14" s="2"/>
       <c r="L14" s="2"/>
-      <c r="M14" s="2"/>
-    </row>
-    <row r="15" customFormat="false" ht="17" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F15" s="38" t="s">
-        <v>5</v>
-      </c>
-      <c r="G15" s="28" t="n">
+    </row>
+    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F15" s="32" t="s">
+        <v>4</v>
+      </c>
+      <c r="G15" s="33" t="n">
         <f aca="false">SUM(G5:G14)</f>
         <v>90</v>
       </c>
-      <c r="H15" s="28" t="n">
+      <c r="H15" s="33" t="n">
         <f aca="false">SUM(H5:H14)</f>
-        <v>15</v>
-      </c>
-      <c r="I15" s="28" t="n">
-        <f aca="false">SUM(I5:I14)</f>
-        <v>684</v>
-      </c>
-      <c r="J15" s="39" t="n">
-        <f aca="false">SUM(G15:I15)</f>
+        <v>699</v>
+      </c>
+      <c r="I15" s="34" t="n">
+        <f aca="false">SUM(G15:H15)</f>
         <v>789</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="8">
-    <mergeCell ref="G2:I3"/>
+    <mergeCell ref="G2:H3"/>
     <mergeCell ref="B5:B14"/>
     <mergeCell ref="C5:C9"/>
     <mergeCell ref="D5:D9"/>

</xml_diff>